<commit_message>
Add 3x3 layer solver results
</commit_message>
<xml_diff>
--- a/data/tabulate.xlsx
+++ b/data/tabulate.xlsx
@@ -19,9 +19,10 @@
     <sheet name="layer_tabulate" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">layer_tabulate!$A$6:$P$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">tabulate!$A$1:$J$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">tabulate_new!$A$1:$M$207</definedName>
-    <definedName name="layer_tabulate" localSheetId="4">layer_tabulate!$A$6:$F$25</definedName>
+    <definedName name="layer_tabulate" localSheetId="4">layer_tabulate!$A$6:$F$50</definedName>
     <definedName name="tabulate" localSheetId="1">tabulate!$A$1:$F$20</definedName>
     <definedName name="tabulate_new" localSheetId="2">tabulate_new!$A$1:$M$207</definedName>
   </definedNames>
@@ -44,7 +45,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="layer_tabulate" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/john/ex/twenty_48/data/layer_tabulate.csv" tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/john/ex/twenty_48/data/layer_tabulate.csv" tab="0" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -91,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="45">
   <si>
     <t>board_size</t>
   </si>
@@ -277,7 +278,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -11288,11 +11299,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:M207"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" activeCellId="1" sqref="H1:H1048576 M1:M1048576"/>
+    <sheetView topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="M195" sqref="M195:M196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11353,7 +11363,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -11394,7 +11404,7 @@
         <v>19.524148602089799</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11435,7 +11445,7 @@
         <v>19.524148732981399</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -11517,7 +11527,7 @@
         <v>19.524148602089799</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -11599,7 +11609,7 @@
         <v>19.524148732981399</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -11681,7 +11691,7 @@
         <v>19.524148732981399</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -11722,7 +11732,7 @@
         <v>19.524148602089799</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -11763,7 +11773,7 @@
         <v>19.524148602089799</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -11804,7 +11814,7 @@
         <v>19.524148732981399</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -11845,7 +11855,7 @@
         <v>19.524148732981399</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -11886,7 +11896,7 @@
         <v>17.172662066258798</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -11927,7 +11937,7 @@
         <v>17.172662527543501</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -11968,7 +11978,7 @@
         <v>17.172663206253102</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -12050,7 +12060,7 @@
         <v>17.172658869852</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -12132,7 +12142,7 @@
         <v>17.172659436188599</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -12214,7 +12224,7 @@
         <v>17.172659436188599</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -12255,7 +12265,7 @@
         <v>17.172662066258798</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -12296,7 +12306,7 @@
         <v>17.172658869852</v>
       </c>
     </row>
-    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -12337,7 +12347,7 @@
         <v>17.172662527543501</v>
       </c>
     </row>
-    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -12378,7 +12388,7 @@
         <v>17.172659436188599</v>
       </c>
     </row>
-    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -12419,7 +12429,7 @@
         <v>17.172663206253102</v>
       </c>
     </row>
-    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -12460,7 +12470,7 @@
         <v>17.172659436188599</v>
       </c>
     </row>
-    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -12501,7 +12511,7 @@
         <v>13.1388608959672</v>
       </c>
     </row>
-    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -12542,7 +12552,7 @@
         <v>13.138860946243</v>
       </c>
     </row>
-    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -12583,7 +12593,7 @@
         <v>13.1388630685107</v>
       </c>
     </row>
-    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -12624,7 +12634,7 @@
         <v>13.138863213131501</v>
       </c>
     </row>
-    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
@@ -12706,7 +12716,7 @@
         <v>13.1388552623348</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
@@ -12788,7 +12798,7 @@
         <v>13.138855342106099</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2</v>
       </c>
@@ -12870,7 +12880,7 @@
         <v>13.138856024610099</v>
       </c>
     </row>
-    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2</v>
       </c>
@@ -12952,7 +12962,7 @@
         <v>13.1388555593707</v>
       </c>
     </row>
-    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
@@ -12993,7 +13003,7 @@
         <v>13.1388608959672</v>
       </c>
     </row>
-    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2</v>
       </c>
@@ -13034,7 +13044,7 @@
         <v>13.1388552623348</v>
       </c>
     </row>
-    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2</v>
       </c>
@@ -13075,7 +13085,7 @@
         <v>13.138860946243</v>
       </c>
     </row>
-    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
@@ -13116,7 +13126,7 @@
         <v>13.138855342106099</v>
       </c>
     </row>
-    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2</v>
       </c>
@@ -13157,7 +13167,7 @@
         <v>13.1388630685107</v>
       </c>
     </row>
-    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2</v>
       </c>
@@ -13198,7 +13208,7 @@
         <v>13.138856024610099</v>
       </c>
     </row>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -13239,7 +13249,7 @@
         <v>13.138863213131501</v>
       </c>
     </row>
-    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -13280,7 +13290,7 @@
         <v>13.1388555593707</v>
       </c>
     </row>
-    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2</v>
       </c>
@@ -13321,7 +13331,7 @@
         <v>0.80614417603335997</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -13362,7 +13372,7 @@
         <v>0.80614417603335997</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2</v>
       </c>
@@ -13403,7 +13413,7 @@
         <v>0.80614416037836001</v>
       </c>
     </row>
-    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2</v>
       </c>
@@ -13444,7 +13454,7 @@
         <v>0.80614416027023905</v>
       </c>
     </row>
-    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2</v>
       </c>
@@ -13526,7 +13536,7 @@
         <v>0.80614342732873501</v>
       </c>
     </row>
-    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -13608,7 +13618,7 @@
         <v>0.80614342732873501</v>
       </c>
     </row>
-    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2</v>
       </c>
@@ -13690,7 +13700,7 @@
         <v>0.80614343298809898</v>
       </c>
     </row>
-    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2</v>
       </c>
@@ -13772,7 +13782,7 @@
         <v>0.80614343265390898</v>
       </c>
     </row>
-    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2</v>
       </c>
@@ -13813,7 +13823,7 @@
         <v>0.80614417603335997</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2</v>
       </c>
@@ -13854,7 +13864,7 @@
         <v>0.80614342732873501</v>
       </c>
     </row>
-    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2</v>
       </c>
@@ -13895,7 +13905,7 @@
         <v>0.80614417603335997</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2</v>
       </c>
@@ -13936,7 +13946,7 @@
         <v>0.80614342732873501</v>
       </c>
     </row>
-    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2</v>
       </c>
@@ -13977,7 +13987,7 @@
         <v>0.80614416037836001</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2</v>
       </c>
@@ -14018,7 +14028,7 @@
         <v>0.80614343298809898</v>
       </c>
     </row>
-    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2</v>
       </c>
@@ -14059,7 +14069,7 @@
         <v>0.80614416027023905</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2</v>
       </c>
@@ -14100,7 +14110,7 @@
         <v>0.80614343265390898</v>
       </c>
     </row>
-    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2</v>
       </c>
@@ -14141,7 +14151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2</v>
       </c>
@@ -14182,7 +14192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2</v>
       </c>
@@ -14223,7 +14233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2</v>
       </c>
@@ -14264,7 +14274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2</v>
       </c>
@@ -14346,7 +14356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2</v>
       </c>
@@ -14428,7 +14438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2</v>
       </c>
@@ -14510,7 +14520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2</v>
       </c>
@@ -14592,7 +14602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2</v>
       </c>
@@ -14633,7 +14643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2</v>
       </c>
@@ -14674,7 +14684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2</v>
       </c>
@@ -14715,7 +14725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2</v>
       </c>
@@ -14756,7 +14766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2</v>
       </c>
@@ -14797,7 +14807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2</v>
       </c>
@@ -14838,7 +14848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2</v>
       </c>
@@ -14879,7 +14889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2</v>
       </c>
@@ -14920,7 +14930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2</v>
       </c>
@@ -14961,7 +14971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2</v>
       </c>
@@ -15002,7 +15012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2</v>
       </c>
@@ -15043,7 +15053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2</v>
       </c>
@@ -15084,7 +15094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2</v>
       </c>
@@ -15166,7 +15176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2</v>
       </c>
@@ -15248,7 +15258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2</v>
       </c>
@@ -15330,7 +15340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2</v>
       </c>
@@ -15412,7 +15422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2</v>
       </c>
@@ -15453,7 +15463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2</v>
       </c>
@@ -15494,7 +15504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2</v>
       </c>
@@ -15535,7 +15545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2</v>
       </c>
@@ -15576,7 +15586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2</v>
       </c>
@@ -15617,7 +15627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2</v>
       </c>
@@ -15658,7 +15668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2</v>
       </c>
@@ -15699,7 +15709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2</v>
       </c>
@@ -15740,7 +15750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>3</v>
       </c>
@@ -15781,7 +15791,7 @@
         <v>19.592127369314301</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>3</v>
       </c>
@@ -15822,7 +15832,7 @@
         <v>19.592124861018998</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>3</v>
       </c>
@@ -15863,7 +15873,7 @@
         <v>19.592127369314301</v>
       </c>
     </row>
-    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>3</v>
       </c>
@@ -15904,7 +15914,7 @@
         <v>19.592124792901899</v>
       </c>
     </row>
-    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>3</v>
       </c>
@@ -15945,7 +15955,7 @@
         <v>19.592124861018998</v>
       </c>
     </row>
-    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>3</v>
       </c>
@@ -15986,7 +15996,7 @@
         <v>19.592124861018998</v>
       </c>
     </row>
-    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>3</v>
       </c>
@@ -16027,7 +16037,7 @@
         <v>19.592127369314301</v>
       </c>
     </row>
-    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>3</v>
       </c>
@@ -16068,7 +16078,7 @@
         <v>19.592124792901899</v>
       </c>
     </row>
-    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>3</v>
       </c>
@@ -16109,7 +16119,7 @@
         <v>19.592124861018998</v>
       </c>
     </row>
-    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>3</v>
       </c>
@@ -16150,7 +16160,7 @@
         <v>19.592124861018998</v>
       </c>
     </row>
-    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>3</v>
       </c>
@@ -16191,7 +16201,7 @@
         <v>17.027650692376699</v>
       </c>
     </row>
-    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>3</v>
       </c>
@@ -16232,7 +16242,7 @@
         <v>17.027649941876799</v>
       </c>
     </row>
-    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>3</v>
       </c>
@@ -16273,7 +16283,7 @@
         <v>17.027649080126899</v>
       </c>
     </row>
-    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>3</v>
       </c>
@@ -16314,7 +16324,7 @@
         <v>17.027650692376699</v>
       </c>
     </row>
-    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>3</v>
       </c>
@@ -16355,7 +16365,7 @@
         <v>17.027643040701602</v>
       </c>
     </row>
-    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>3</v>
       </c>
@@ -16396,7 +16406,7 @@
         <v>17.027649941876799</v>
       </c>
     </row>
-    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>3</v>
       </c>
@@ -16437,7 +16447,7 @@
         <v>17.027643400038901</v>
       </c>
     </row>
-    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>3</v>
       </c>
@@ -16478,7 +16488,7 @@
         <v>17.027649080126899</v>
       </c>
     </row>
-    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>3</v>
       </c>
@@ -16519,7 +16529,7 @@
         <v>17.027643690642702</v>
       </c>
     </row>
-    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>3</v>
       </c>
@@ -16560,7 +16570,7 @@
         <v>17.027650692376699</v>
       </c>
     </row>
-    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>3</v>
       </c>
@@ -16601,7 +16611,7 @@
         <v>17.027643040701602</v>
       </c>
     </row>
-    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>3</v>
       </c>
@@ -16642,7 +16652,7 @@
         <v>17.027649941876799</v>
       </c>
     </row>
-    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>3</v>
       </c>
@@ -16683,7 +16693,7 @@
         <v>17.027643400038901</v>
       </c>
     </row>
-    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>3</v>
       </c>
@@ -16724,7 +16734,7 @@
         <v>17.027649080126899</v>
       </c>
     </row>
-    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>3</v>
       </c>
@@ -16765,7 +16775,7 @@
         <v>17.027643690642702</v>
       </c>
     </row>
-    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>3</v>
       </c>
@@ -16806,7 +16816,7 @@
         <v>13.2392119041229</v>
       </c>
     </row>
-    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>3</v>
       </c>
@@ -16847,7 +16857,7 @@
         <v>13.239211860137701</v>
       </c>
     </row>
-    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>3</v>
       </c>
@@ -16888,7 +16898,7 @@
         <v>13.239210639912701</v>
       </c>
     </row>
-    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>3</v>
       </c>
@@ -16929,7 +16939,7 @@
         <v>13.238491440254601</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>3</v>
       </c>
@@ -16970,7 +16980,7 @@
         <v>13.2392119041229</v>
       </c>
     </row>
-    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>3</v>
       </c>
@@ -17011,7 +17021,7 @@
         <v>13.2391984807368</v>
       </c>
     </row>
-    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>3</v>
       </c>
@@ -17052,7 +17062,7 @@
         <v>13.239211860137701</v>
       </c>
     </row>
-    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>3</v>
       </c>
@@ -17093,7 +17103,7 @@
         <v>13.2391987940783</v>
       </c>
     </row>
-    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>3</v>
       </c>
@@ -17134,7 +17144,7 @@
         <v>13.239210639912701</v>
       </c>
     </row>
-    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>3</v>
       </c>
@@ -17175,7 +17185,7 @@
         <v>13.2391992002153</v>
       </c>
     </row>
-    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>3</v>
       </c>
@@ -17216,7 +17226,7 @@
         <v>13.2384909299761</v>
       </c>
     </row>
-    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>3</v>
       </c>
@@ -17257,7 +17267,7 @@
         <v>13.238478895600601</v>
       </c>
     </row>
-    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>3</v>
       </c>
@@ -17298,7 +17308,7 @@
         <v>13.2392119041229</v>
       </c>
     </row>
-    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>3</v>
       </c>
@@ -17339,7 +17349,7 @@
         <v>13.2391984807368</v>
       </c>
     </row>
-    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>3</v>
       </c>
@@ -17380,7 +17390,7 @@
         <v>13.239211860137701</v>
       </c>
     </row>
-    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>3</v>
       </c>
@@ -17421,7 +17431,7 @@
         <v>13.2391987940783</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>3</v>
       </c>
@@ -17462,7 +17472,7 @@
         <v>13.239210639912701</v>
       </c>
     </row>
-    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>3</v>
       </c>
@@ -17503,7 +17513,7 @@
         <v>13.2391992002153</v>
       </c>
     </row>
-    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>3</v>
       </c>
@@ -17544,7 +17554,7 @@
         <v>13.2384910246099</v>
       </c>
     </row>
-    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>3</v>
       </c>
@@ -17585,7 +17595,7 @@
         <v>13.238478895112699</v>
       </c>
     </row>
-    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>3</v>
       </c>
@@ -17626,7 +17636,7 @@
         <v>8.5913877502300409</v>
       </c>
     </row>
-    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>3</v>
       </c>
@@ -17667,7 +17677,7 @@
         <v>8.5913877475085201</v>
       </c>
     </row>
-    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>3</v>
       </c>
@@ -17708,7 +17718,7 @@
         <v>8.5913877308337607</v>
       </c>
     </row>
-    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>3</v>
       </c>
@@ -17749,7 +17759,7 @@
         <v>8.5913874927204805</v>
       </c>
     </row>
-    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>3</v>
       </c>
@@ -17790,7 +17800,7 @@
         <v>8.5913877502300409</v>
       </c>
     </row>
-    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>3</v>
       </c>
@@ -17831,7 +17841,7 @@
         <v>8.5913755575086306</v>
       </c>
     </row>
-    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>3</v>
       </c>
@@ -17872,7 +17882,7 @@
         <v>8.5913877475085201</v>
       </c>
     </row>
-    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>3</v>
       </c>
@@ -17913,7 +17923,7 @@
         <v>8.5913757864995706</v>
       </c>
     </row>
-    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>3</v>
       </c>
@@ -17954,7 +17964,7 @@
         <v>8.5913877308337607</v>
       </c>
     </row>
-    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>3</v>
       </c>
@@ -17995,7 +18005,7 @@
         <v>8.5913760284402994</v>
       </c>
     </row>
-    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>3</v>
       </c>
@@ -18036,7 +18046,7 @@
         <v>8.5913877502300409</v>
       </c>
     </row>
-    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>3</v>
       </c>
@@ -18077,7 +18087,7 @@
         <v>8.5913755575086306</v>
       </c>
     </row>
-    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>3</v>
       </c>
@@ -18118,7 +18128,7 @@
         <v>8.5913877475085201</v>
       </c>
     </row>
-    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>3</v>
       </c>
@@ -18159,7 +18169,7 @@
         <v>8.5913757864995706</v>
       </c>
     </row>
-    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>3</v>
       </c>
@@ -18200,7 +18210,7 @@
         <v>8.5913877308337607</v>
       </c>
     </row>
-    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>3</v>
       </c>
@@ -18241,7 +18251,7 @@
         <v>8.5913760284402994</v>
       </c>
     </row>
-    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>3</v>
       </c>
@@ -18282,7 +18292,7 @@
         <v>8.5913874829357901</v>
       </c>
     </row>
-    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>3</v>
       </c>
@@ -18323,7 +18333,7 @@
         <v>8.5913760658561493</v>
       </c>
     </row>
-    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>3</v>
       </c>
@@ -18364,7 +18374,7 @@
         <v>3.8907248974833402</v>
       </c>
     </row>
-    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>3</v>
       </c>
@@ -18405,7 +18415,7 @@
         <v>3.8907249702630802</v>
       </c>
     </row>
-    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>3</v>
       </c>
@@ -18446,7 +18456,7 @@
         <v>3.8907161364825602</v>
       </c>
     </row>
-    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>3</v>
       </c>
@@ -18487,7 +18497,7 @@
         <v>3.89072489749682</v>
       </c>
     </row>
-    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>3</v>
       </c>
@@ -18528,7 +18538,7 @@
         <v>3.8907249702630802</v>
       </c>
     </row>
-    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>3</v>
       </c>
@@ -18569,7 +18579,7 @@
         <v>3.8907162725952</v>
       </c>
     </row>
-    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>3</v>
       </c>
@@ -18610,7 +18620,7 @@
         <v>3.89072489749217</v>
       </c>
     </row>
-    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>3</v>
       </c>
@@ -18651,7 +18661,7 @@
         <v>3.8907249702630802</v>
       </c>
     </row>
-    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>3</v>
       </c>
@@ -18692,7 +18702,7 @@
         <v>3.8907164160785199</v>
       </c>
     </row>
-    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>3</v>
       </c>
@@ -18733,7 +18743,7 @@
         <v>3.8907248974833402</v>
       </c>
     </row>
-    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>3</v>
       </c>
@@ -18774,7 +18784,7 @@
         <v>3.8907249702630802</v>
       </c>
     </row>
-    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>3</v>
       </c>
@@ -18815,7 +18825,7 @@
         <v>3.8907161364825602</v>
       </c>
     </row>
-    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>3</v>
       </c>
@@ -18856,7 +18866,7 @@
         <v>3.89072489749682</v>
       </c>
     </row>
-    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>3</v>
       </c>
@@ -18897,7 +18907,7 @@
         <v>3.8898473598413199</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>3</v>
       </c>
@@ -18938,7 +18948,7 @@
         <v>3.8907162725952</v>
       </c>
     </row>
-    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>3</v>
       </c>
@@ -18979,7 +18989,7 @@
         <v>3.89072489749217</v>
       </c>
     </row>
-    <row r="188" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>3</v>
       </c>
@@ -19020,7 +19030,7 @@
         <v>3.8898618151459301</v>
       </c>
     </row>
-    <row r="189" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>3</v>
       </c>
@@ -19061,7 +19071,7 @@
         <v>3.8907164160785199</v>
       </c>
     </row>
-    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>3</v>
       </c>
@@ -19102,7 +19112,7 @@
         <v>3.8907249640427901</v>
       </c>
     </row>
-    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>3</v>
       </c>
@@ -19143,7 +19153,7 @@
         <v>3.8898771468932698</v>
       </c>
     </row>
-    <row r="192" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>3</v>
       </c>
@@ -19184,7 +19194,7 @@
         <v>3.8907165672874799</v>
       </c>
     </row>
-    <row r="193" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>3</v>
       </c>
@@ -19225,7 +19235,7 @@
         <v>0.83719564085741105</v>
       </c>
     </row>
-    <row r="194" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>3</v>
       </c>
@@ -19266,7 +19276,7 @@
         <v>4.0312572363225198E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>3</v>
       </c>
@@ -19307,7 +19317,7 @@
         <v>4.0312570668023601E-2</v>
       </c>
     </row>
-    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>3</v>
       </c>
@@ -19348,7 +19358,7 @@
         <v>4.0312569166368703E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>4</v>
       </c>
@@ -19389,7 +19399,7 @@
         <v>19.571784533368099</v>
       </c>
     </row>
-    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>4</v>
       </c>
@@ -19430,7 +19440,7 @@
         <v>19.571782022561901</v>
       </c>
     </row>
-    <row r="199" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>4</v>
       </c>
@@ -19471,7 +19481,7 @@
         <v>19.571784533368</v>
       </c>
     </row>
-    <row r="200" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>4</v>
       </c>
@@ -19512,7 +19522,7 @@
         <v>19.571782022561798</v>
       </c>
     </row>
-    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>4</v>
       </c>
@@ -19553,7 +19563,7 @@
         <v>16.940706392439701</v>
       </c>
     </row>
-    <row r="202" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>4</v>
       </c>
@@ -19594,7 +19604,7 @@
         <v>16.940705814110402</v>
       </c>
     </row>
-    <row r="203" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>4</v>
       </c>
@@ -19635,7 +19645,7 @@
         <v>16.940704707611602</v>
       </c>
     </row>
-    <row r="204" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>4</v>
       </c>
@@ -19676,7 +19686,7 @@
         <v>16.940706392439701</v>
       </c>
     </row>
-    <row r="205" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>4</v>
       </c>
@@ -19717,7 +19727,7 @@
         <v>16.9407050038417</v>
       </c>
     </row>
-    <row r="206" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>4</v>
       </c>
@@ -19758,7 +19768,7 @@
         <v>16.940704707611602</v>
       </c>
     </row>
-    <row r="207" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>4</v>
       </c>
@@ -19800,23 +19810,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M207">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="2"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="exact"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="value_iteration"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -20206,10 +20199,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20218,7 +20211,7 @@
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.1640625" customWidth="1"/>
@@ -20366,19 +20359,19 @@
         <v>0.85863380508680498</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G25" si="0">F8*20</f>
+        <f t="shared" ref="G8:G50" si="0">F8*20</f>
         <v>17.172676101736101</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:H25" si="1">E8+2</f>
+        <f t="shared" ref="H8:H49" si="1">E8+2</f>
         <v>13</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I25" si="2">ABS(G8-P8)</f>
+        <f t="shared" ref="I8:I71" si="2">ABS(G8-P8)</f>
         <v>1.6665547502014988E-5</v>
       </c>
       <c r="J8">
-        <f t="shared" ref="J8:J25" si="3">ABS(H8-O8)</f>
+        <f>ABS(H8-O8)</f>
         <v>0</v>
       </c>
       <c r="K8">
@@ -20432,7 +20425,7 @@
         <v>1.6665547502014988E-5</v>
       </c>
       <c r="J9">
-        <f t="shared" si="3"/>
+        <f>ABS(H9-O9)</f>
         <v>0</v>
       </c>
       <c r="K9">
@@ -20486,7 +20479,7 @@
         <v>1.5236304019339286E-5</v>
       </c>
       <c r="J10">
-        <f t="shared" si="3"/>
+        <f>ABS(H10-O10)</f>
         <v>0</v>
       </c>
       <c r="K10">
@@ -20540,7 +20533,7 @@
         <v>1.5156532720439486E-5</v>
       </c>
       <c r="J11">
-        <f t="shared" si="3"/>
+        <f>ABS(H11-O11)</f>
         <v>1</v>
       </c>
       <c r="K11">
@@ -20594,7 +20587,7 @@
         <v>1.4474028720457E-5</v>
       </c>
       <c r="J12">
-        <f t="shared" si="3"/>
+        <f>ABS(H12-O12)</f>
         <v>2</v>
       </c>
       <c r="K12">
@@ -20648,7 +20641,7 @@
         <v>1.4939268119462668E-5</v>
       </c>
       <c r="J13">
-        <f t="shared" si="3"/>
+        <f>ABS(H13-O13)</f>
         <v>3</v>
       </c>
       <c r="K13">
@@ -20702,7 +20695,7 @@
         <v>1.0809384969334701E-6</v>
       </c>
       <c r="J14">
-        <f t="shared" si="3"/>
+        <f>ABS(H14-O14)</f>
         <v>0</v>
       </c>
       <c r="K14">
@@ -20756,7 +20749,7 @@
         <v>1.0809384969334701E-6</v>
       </c>
       <c r="J15">
-        <f t="shared" si="3"/>
+        <f>ABS(H15-O15)</f>
         <v>1</v>
       </c>
       <c r="K15">
@@ -20810,7 +20803,7 @@
         <v>1.0752791329560196E-6</v>
       </c>
       <c r="J16">
-        <f t="shared" si="3"/>
+        <f>ABS(H16-O16)</f>
         <v>2</v>
       </c>
       <c r="K16">
@@ -20832,7 +20825,7 @@
         <v>0.80614343298809898</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -20864,7 +20857,7 @@
         <v>1.0756133229650189E-6</v>
       </c>
       <c r="J17">
-        <f t="shared" si="3"/>
+        <f>ABS(H17-O17)</f>
         <v>3</v>
       </c>
       <c r="K17">
@@ -20886,7 +20879,7 @@
         <v>0.80614343265390898</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -20918,7 +20911,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <f t="shared" si="3"/>
+        <f>ABS(H18-O18)</f>
         <v>1</v>
       </c>
       <c r="K18">
@@ -20940,7 +20933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -20972,7 +20965,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <f t="shared" si="3"/>
+        <f>ABS(H19-O19)</f>
         <v>1</v>
       </c>
       <c r="K19">
@@ -20994,7 +20987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -21026,7 +21019,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <f t="shared" si="3"/>
+        <f>ABS(H20-O20)</f>
         <v>1</v>
       </c>
       <c r="K20">
@@ -21048,7 +21041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -21080,7 +21073,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <f t="shared" si="3"/>
+        <f>ABS(H21-O21)</f>
         <v>1</v>
       </c>
       <c r="K21">
@@ -21102,7 +21095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -21134,7 +21127,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <f t="shared" si="3"/>
+        <f>ABS(H22-O22)</f>
         <v>1</v>
       </c>
       <c r="K22">
@@ -21156,7 +21149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -21188,7 +21181,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <f t="shared" si="3"/>
+        <f>ABS(H23-O23)</f>
         <v>1</v>
       </c>
       <c r="K23">
@@ -21210,7 +21203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -21242,7 +21235,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <f t="shared" si="3"/>
+        <f>ABS(H24-O24)</f>
         <v>1</v>
       </c>
       <c r="K24">
@@ -21264,7 +21257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -21296,31 +21289,1243 @@
         <v>0</v>
       </c>
       <c r="J25">
+        <f>ABS(H25-O25)</f>
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+      <c r="L25">
+        <v>7</v>
+      </c>
+      <c r="M25" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25">
+        <v>3</v>
+      </c>
+      <c r="O25">
+        <v>71</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0.95</v>
+      </c>
+      <c r="E26">
+        <v>1186</v>
+      </c>
+      <c r="F26">
+        <v>0.85138298515770605</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>17.027659703154121</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>1188</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>1.6662452519966564E-5</v>
+      </c>
+      <c r="J26">
+        <f t="shared" ref="J26:J47" si="3">ABS(H26-O26)</f>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>3</v>
+      </c>
+      <c r="L26">
+        <v>3</v>
+      </c>
+      <c r="M26" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>1188</v>
+      </c>
+      <c r="P26">
+        <v>17.027643040701602</v>
+      </c>
+      <c r="Q26" s="4"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0.95</v>
+      </c>
+      <c r="E27">
+        <v>356</v>
+      </c>
+      <c r="F27">
+        <v>0.85138298515770605</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="0"/>
+        <v>17.027659703154121</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>358</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>1.6303115220495101E-5</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
+      <c r="L27">
+        <v>3</v>
+      </c>
+      <c r="M27" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>355</v>
+      </c>
+      <c r="P27">
+        <v>17.027643400038901</v>
+      </c>
+      <c r="Q27" s="4"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>0.95</v>
+      </c>
+      <c r="E28">
+        <v>99</v>
+      </c>
+      <c r="F28">
+        <v>0.85120279622033201</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>17.024055924406639</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>3.5877662360626061E-3</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="K28">
+        <v>3</v>
+      </c>
+      <c r="L28">
+        <v>3</v>
+      </c>
+      <c r="M28" t="s">
+        <v>22</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28">
+        <v>96</v>
+      </c>
+      <c r="P28">
+        <v>17.027643690642702</v>
+      </c>
+      <c r="Q28" s="4"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0.95</v>
+      </c>
+      <c r="E29">
+        <v>16834</v>
+      </c>
+      <c r="F29">
+        <v>0.66196066943017196</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="0"/>
+        <v>13.239213388603439</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>16836</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>1.4907866638935729E-5</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <v>4</v>
+      </c>
+      <c r="M29" t="s">
+        <v>22</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>16836</v>
+      </c>
+      <c r="P29">
+        <v>13.2391984807368</v>
+      </c>
+      <c r="Q29" s="4"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0.95</v>
+      </c>
+      <c r="E30">
+        <v>9828</v>
+      </c>
+      <c r="F30">
+        <v>0.66196066943017196</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="0"/>
+        <v>13.239213388603439</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>9830</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>1.4594525138633685E-5</v>
+      </c>
+      <c r="J30">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="K25">
-        <v>2</v>
-      </c>
-      <c r="L25">
+      <c r="K30">
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <v>4</v>
+      </c>
+      <c r="M30" t="s">
+        <v>22</v>
+      </c>
+      <c r="N30">
+        <v>1</v>
+      </c>
+      <c r="O30">
+        <v>9831</v>
+      </c>
+      <c r="P30">
+        <v>13.2391987940783</v>
+      </c>
+      <c r="Q30" s="4"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>0.95</v>
+      </c>
+      <c r="E31">
+        <v>4596</v>
+      </c>
+      <c r="F31">
+        <v>0.66196066943017196</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="0"/>
+        <v>13.239213388603439</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>4598</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>1.4188388139046992E-5</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <v>3</v>
+      </c>
+      <c r="L31">
+        <v>4</v>
+      </c>
+      <c r="M31" t="s">
+        <v>22</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+      <c r="O31">
+        <v>4600</v>
+      </c>
+      <c r="P31">
+        <v>13.2391992002153</v>
+      </c>
+      <c r="Q31" s="4"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>0.95</v>
+      </c>
+      <c r="E32">
+        <v>1984</v>
+      </c>
+      <c r="F32">
+        <v>0.66191975073806797</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="0"/>
+        <v>13.238395014761359</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>1986</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="2"/>
+        <v>8.3880839241601279E-5</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="K32">
+        <v>3</v>
+      </c>
+      <c r="L32">
+        <v>4</v>
+      </c>
+      <c r="M32" t="s">
+        <v>22</v>
+      </c>
+      <c r="N32">
+        <v>3</v>
+      </c>
+      <c r="O32">
+        <v>2018</v>
+      </c>
+      <c r="P32">
+        <v>13.238478895600601</v>
+      </c>
+      <c r="Q32" s="4"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0.95</v>
+      </c>
+      <c r="E33">
+        <v>124372</v>
+      </c>
+      <c r="F33">
+        <v>0.42956939062997401</v>
+      </c>
+      <c r="G33">
+        <f>F33*20</f>
+        <v>8.5913878125994803</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>124374</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="2"/>
+        <v>1.2255090849677686E-5</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>3</v>
+      </c>
+      <c r="L33">
+        <v>5</v>
+      </c>
+      <c r="M33" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>124374</v>
+      </c>
+      <c r="P33">
+        <v>8.5913755575086306</v>
+      </c>
+      <c r="Q33" s="4"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0.95</v>
+      </c>
+      <c r="E34">
+        <v>92076</v>
+      </c>
+      <c r="F34">
+        <v>0.42956939062997401</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="0"/>
+        <v>8.5913878125994803</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>92078</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="2"/>
+        <v>1.2026099909689947E-5</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>3</v>
+      </c>
+      <c r="L34">
+        <v>5</v>
+      </c>
+      <c r="M34" t="s">
+        <v>22</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>92079</v>
+      </c>
+      <c r="P34">
+        <v>8.5913757864995706</v>
+      </c>
+      <c r="Q34" s="4"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>0.95</v>
+      </c>
+      <c r="E35">
+        <v>65897</v>
+      </c>
+      <c r="F35">
+        <v>0.42956939062997401</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="0"/>
+        <v>8.5913878125994803</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>65899</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>1.1784159180905363E-5</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K35">
+        <v>3</v>
+      </c>
+      <c r="L35">
+        <v>5</v>
+      </c>
+      <c r="M35" t="s">
+        <v>22</v>
+      </c>
+      <c r="N35">
+        <v>2</v>
+      </c>
+      <c r="O35">
+        <v>65901</v>
+      </c>
+      <c r="P35">
+        <v>8.5913760284402994</v>
+      </c>
+      <c r="Q35" s="4"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0.95</v>
+      </c>
+      <c r="E36">
+        <v>594046</v>
+      </c>
+      <c r="F36">
+        <v>0.19453624851315501</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="0"/>
+        <v>3.8907249702631002</v>
+      </c>
+      <c r="H36">
+        <f>E36+2</f>
+        <v>594048</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="2"/>
+        <v>8.8337805399518743E-6</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>3</v>
+      </c>
+      <c r="L36">
+        <v>6</v>
+      </c>
+      <c r="M36" t="s">
+        <v>22</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>594048</v>
+      </c>
+      <c r="P36">
+        <v>3.8907161364825602</v>
+      </c>
+      <c r="Q36" s="4"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0.95</v>
+      </c>
+      <c r="E37">
+        <v>489025</v>
+      </c>
+      <c r="F37">
+        <v>0.19453624851315501</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="0"/>
+        <v>3.8907249702631002</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>489027</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>8.6976679001260493E-6</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>3</v>
+      </c>
+      <c r="L37">
+        <v>6</v>
+      </c>
+      <c r="M37" t="s">
+        <v>22</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>489028</v>
+      </c>
+      <c r="P37">
+        <v>3.8907162725952</v>
+      </c>
+      <c r="Q37" s="4"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>0.95</v>
+      </c>
+      <c r="E38">
+        <v>405126</v>
+      </c>
+      <c r="F38">
+        <v>0.19453624851315501</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="0"/>
+        <v>3.8907249702631002</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="1"/>
+        <v>405128</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>8.5541845802339367E-6</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K38">
+        <v>3</v>
+      </c>
+      <c r="L38">
+        <v>6</v>
+      </c>
+      <c r="M38" t="s">
+        <v>22</v>
+      </c>
+      <c r="N38">
+        <v>2</v>
+      </c>
+      <c r="O38">
+        <v>405130</v>
+      </c>
+      <c r="P38">
+        <v>3.8907164160785199</v>
+      </c>
+      <c r="Q38" s="4"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
         <v>7</v>
       </c>
-      <c r="M25" t="s">
-        <v>22</v>
-      </c>
-      <c r="N25">
-        <v>3</v>
-      </c>
-      <c r="O25">
-        <v>71</v>
-      </c>
-      <c r="P25">
-        <v>0</v>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0.95</v>
+      </c>
+      <c r="E39">
+        <v>2064918</v>
+      </c>
+      <c r="F39">
+        <v>4.18598094971964E-2</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="0"/>
+        <v>0.83719618994392797</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>2064920</v>
+      </c>
+      <c r="I39">
+        <f t="shared" ref="I39:I50" si="4">ABS(G39-P39)</f>
+        <v>5.4908651692109345E-7</v>
+      </c>
+      <c r="J39">
+        <f t="shared" ref="J39:J50" si="5">ABS(H39-O39)</f>
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>3</v>
+      </c>
+      <c r="L39">
+        <v>7</v>
+      </c>
+      <c r="M39" t="s">
+        <v>23</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>2064920</v>
+      </c>
+      <c r="P39">
+        <v>0.83719564085741105</v>
+      </c>
+      <c r="Q39" s="4"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>7</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>0.95</v>
+      </c>
+      <c r="E40">
+        <v>1813775</v>
+      </c>
+      <c r="F40">
+        <v>4.18598094971964E-2</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="0"/>
+        <v>0.83719618994392797</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>1813777</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="4"/>
+        <v>0.83719618994392797</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="5"/>
+        <v>1813777</v>
+      </c>
+      <c r="Q40" s="4"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>0.95</v>
+      </c>
+      <c r="E41">
+        <v>1618957</v>
+      </c>
+      <c r="F41">
+        <v>4.18598094971964E-2</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="0"/>
+        <v>0.83719618994392797</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>1618959</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="4"/>
+        <v>0.83719618994392797</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="5"/>
+        <v>1618959</v>
+      </c>
+      <c r="Q41" s="4"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0.95</v>
+      </c>
+      <c r="E42">
+        <v>5643584</v>
+      </c>
+      <c r="F42">
+        <v>2.0156432845151902E-3</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="0"/>
+        <v>4.0312865690303804E-2</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>5643586</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="4"/>
+        <v>4.0312865690303804E-2</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="5"/>
+        <v>5643586</v>
+      </c>
+      <c r="Q42" s="4"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>0.95</v>
+      </c>
+      <c r="E43">
+        <v>5161162</v>
+      </c>
+      <c r="F43">
+        <v>2.0156432845151902E-3</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="0"/>
+        <v>4.0312865690303804E-2</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>5161164</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="4"/>
+        <v>2.9332707860568741E-7</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>3</v>
+      </c>
+      <c r="L43">
+        <v>8</v>
+      </c>
+      <c r="M43" t="s">
+        <v>23</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>5161165</v>
+      </c>
+      <c r="P43">
+        <v>4.0312572363225198E-2</v>
+      </c>
+      <c r="Q43" s="4"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>0.95</v>
+      </c>
+      <c r="E44">
+        <v>4797076</v>
+      </c>
+      <c r="F44">
+        <v>2.0156432845151902E-3</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="0"/>
+        <v>4.0312865690303804E-2</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="1"/>
+        <v>4797078</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="4"/>
+        <v>2.9502228020283905E-7</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K44">
+        <v>3</v>
+      </c>
+      <c r="L44">
+        <v>8</v>
+      </c>
+      <c r="M44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N44">
+        <v>2</v>
+      </c>
+      <c r="O44">
+        <v>4797080</v>
+      </c>
+      <c r="P44">
+        <v>4.0312570668023601E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>9</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0.95</v>
+      </c>
+      <c r="E45">
+        <v>12789511</v>
+      </c>
+      <c r="F45" s="4">
+        <v>3.7091897410257201E-6</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="0"/>
+        <v>7.4183794820514409E-5</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="1"/>
+        <v>12789513</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="4"/>
+        <v>7.4183794820514409E-5</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="5"/>
+        <v>12789513</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46">
+        <v>9</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>0.95</v>
+      </c>
+      <c r="E46">
+        <v>12013249</v>
+      </c>
+      <c r="F46" s="4">
+        <v>3.7091897410257201E-6</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="0"/>
+        <v>7.4183794820514409E-5</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>12013251</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="4"/>
+        <v>7.4183794820514409E-5</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="5"/>
+        <v>12013251</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>9</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>0.95</v>
+      </c>
+      <c r="E47">
+        <v>11413938</v>
+      </c>
+      <c r="F47" s="4">
+        <v>3.7091897410257201E-6</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="0"/>
+        <v>7.4183794820514409E-5</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="1"/>
+        <v>11413940</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="4"/>
+        <v>7.4183794820514409E-5</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="5"/>
+        <v>11413940</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0.95</v>
+      </c>
+      <c r="E48">
+        <v>25179012</v>
+      </c>
+      <c r="F48" s="4">
+        <v>3.7321372076390899E-13</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="0"/>
+        <v>7.4642744152781792E-12</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="1"/>
+        <v>25179014</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="4"/>
+        <v>7.4642744152781792E-12</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="5"/>
+        <v>25179014</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49">
+        <v>0.95</v>
+      </c>
+      <c r="E49">
+        <v>23939949</v>
+      </c>
+      <c r="F49" s="4">
+        <v>3.7321372076390899E-13</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="0"/>
+        <v>7.4642744152781792E-12</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="1"/>
+        <v>23939951</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="4"/>
+        <v>7.4642744152781792E-12</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="5"/>
+        <v>23939951</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>0.95</v>
+      </c>
+      <c r="E50">
+        <v>22994914</v>
+      </c>
+      <c r="F50" s="4">
+        <v>3.7321372076390899E-13</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="0"/>
+        <v>7.4642744152781792E-12</v>
+      </c>
+      <c r="H50">
+        <f>E50+2</f>
+        <v>22994916</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="4"/>
+        <v>7.4642744152781792E-12</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="5"/>
+        <v>22994916</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I7:I25">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+  <autoFilter ref="A6:P50">
+    <sortState ref="A7:P50">
+      <sortCondition ref="A7:A50"/>
+      <sortCondition ref="B7:B50"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="I7:I102">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0.0001</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix valuing of mixed known and unknown successors
</commit_message>
<xml_diff>
--- a/data/tabulate.xlsx
+++ b/data/tabulate.xlsx
@@ -9,27 +9,30 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="tabulate" sheetId="1" r:id="rId2"/>
     <sheet name="tabulate_new" sheetId="3" r:id="rId3"/>
-    <sheet name="pivot" sheetId="4" r:id="rId4"/>
-    <sheet name="layer_tabulate" sheetId="5" r:id="rId5"/>
+    <sheet name="tabulate_native" sheetId="6" r:id="rId4"/>
+    <sheet name="pivot" sheetId="4" r:id="rId5"/>
+    <sheet name="layer_tabulate" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">layer_tabulate!$A$6:$P$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">layer_tabulate!$A$6:$Q$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">tabulate!$A$1:$J$87</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">tabulate_native!$A$1:$E$183</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">tabulate_new!$A$1:$M$207</definedName>
-    <definedName name="layer_tabulate" localSheetId="4">layer_tabulate!$A$6:$F$50</definedName>
+    <definedName name="layer_tabulate" localSheetId="5">layer_tabulate!$A$6:$F$50</definedName>
     <definedName name="tabulate" localSheetId="1">tabulate!$A$1:$F$20</definedName>
+    <definedName name="tabulate_native" localSheetId="3">tabulate_native!$A$1:$E$183</definedName>
     <definedName name="tabulate_new" localSheetId="2">tabulate_new!$A$1:$M$207</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="2" r:id="rId7"/>
+    <pivotCache cacheId="3" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -72,8 +75,19 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="tabulate_new" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/john/ex/twenty_48/data/tabulate.csv" tab="0" comma="1">
+  <connection id="3" name="tabulate_native" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" codePage="10000" sourceFile="/Users/john/ex/twenty_48/data/tabulate_native.csv" tab="0" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="tabulate_new" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/john/ex/twenty_48/data/tabulate_native.csv" tab="0" comma="1">
       <textFields count="10">
         <textField/>
         <textField/>
@@ -92,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="48">
   <si>
     <t>board_size</t>
   </si>
@@ -228,6 +242,15 @@
   <si>
     <t>compare layer tabulate results with the ruby model tabulate results</t>
   </si>
+  <si>
+    <t>max_lose_depth</t>
+  </si>
+  <si>
+    <t>max_win_depth</t>
+  </si>
+  <si>
+    <t>native</t>
+  </si>
 </sst>
 </file>
 
@@ -278,37 +301,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3817,7 +3810,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:S13" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
@@ -3958,7 +3951,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:D33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -4216,10 +4209,14 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tabulate_new" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tabulate_new" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tabulate_native" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="layer_tabulate" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -11283,12 +11280,12 @@
   </sheetData>
   <autoFilter ref="A1:J87"/>
   <conditionalFormatting sqref="N2:N87">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y87">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11301,8 +11298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M207"/>
   <sheetViews>
-    <sheetView topLeftCell="A186" workbookViewId="0">
-      <selection activeCell="M195" sqref="M195:M196"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19816,6 +19813,3147 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:E183"/>
+  <sheetViews>
+    <sheetView topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="E136" sqref="E136"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2</v>
+      </c>
+      <c r="B35">
+        <v>5</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>2</v>
+      </c>
+      <c r="B39">
+        <v>6</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>2</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+      <c r="E40">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>2</v>
+      </c>
+      <c r="B41">
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="E43">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2</v>
+      </c>
+      <c r="B44">
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45">
+        <v>6</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>6</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>7</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>7</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="E49">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>7</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <v>7</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2</v>
+      </c>
+      <c r="B55">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+      <c r="E55">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>3</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>2</v>
+      </c>
+      <c r="E61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>3</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>3</v>
+      </c>
+      <c r="B63">
+        <v>2</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>3</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>3</v>
+      </c>
+      <c r="B67">
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+      <c r="E67">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>3</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>3</v>
+      </c>
+      <c r="B70">
+        <v>3</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>3</v>
+      </c>
+      <c r="B71">
+        <v>3</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>3</v>
+      </c>
+      <c r="B72">
+        <v>3</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>3</v>
+      </c>
+      <c r="B73">
+        <v>3</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="E73">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>3</v>
+      </c>
+      <c r="B74">
+        <v>4</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>16836</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>4</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>9831</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>3</v>
+      </c>
+      <c r="B76">
+        <v>4</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>3</v>
+      </c>
+      <c r="B77">
+        <v>4</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>16836</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>3</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>9831</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>3</v>
+      </c>
+      <c r="B79">
+        <v>4</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="E79">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>4</v>
+      </c>
+      <c r="C80">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>16836</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>3</v>
+      </c>
+      <c r="B81">
+        <v>4</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>9831</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>3</v>
+      </c>
+      <c r="B82">
+        <v>4</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+      <c r="E82">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>5</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>124374</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>3</v>
+      </c>
+      <c r="B84">
+        <v>5</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+      <c r="E84">
+        <v>92115</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>3</v>
+      </c>
+      <c r="B85">
+        <v>5</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>2</v>
+      </c>
+      <c r="E85">
+        <v>65944</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>3</v>
+      </c>
+      <c r="B86">
+        <v>5</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>124288</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>3</v>
+      </c>
+      <c r="B87">
+        <v>5</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>92079</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>3</v>
+      </c>
+      <c r="B88">
+        <v>5</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88">
+        <v>65911</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>3</v>
+      </c>
+      <c r="B89">
+        <v>5</v>
+      </c>
+      <c r="C89">
+        <v>2</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>124256</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>3</v>
+      </c>
+      <c r="B90">
+        <v>5</v>
+      </c>
+      <c r="C90">
+        <v>2</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>92067</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>3</v>
+      </c>
+      <c r="B91">
+        <v>5</v>
+      </c>
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91">
+        <v>2</v>
+      </c>
+      <c r="E91">
+        <v>65901</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>3</v>
+      </c>
+      <c r="B92">
+        <v>6</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>594048</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>3</v>
+      </c>
+      <c r="B93">
+        <v>6</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+      <c r="E93">
+        <v>490333</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>3</v>
+      </c>
+      <c r="B94">
+        <v>6</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>2</v>
+      </c>
+      <c r="E94">
+        <v>406956</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>3</v>
+      </c>
+      <c r="B95">
+        <v>6</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>592253</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>3</v>
+      </c>
+      <c r="B96">
+        <v>6</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>489028</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>3</v>
+      </c>
+      <c r="B97">
+        <v>6</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>2</v>
+      </c>
+      <c r="E97">
+        <v>405733</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>3</v>
+      </c>
+      <c r="B98">
+        <v>6</v>
+      </c>
+      <c r="C98">
+        <v>2</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>591376</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>3</v>
+      </c>
+      <c r="B99">
+        <v>6</v>
+      </c>
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>488346</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>3</v>
+      </c>
+      <c r="B100">
+        <v>6</v>
+      </c>
+      <c r="C100">
+        <v>2</v>
+      </c>
+      <c r="D100">
+        <v>2</v>
+      </c>
+      <c r="E100">
+        <v>405130</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>3</v>
+      </c>
+      <c r="B101">
+        <v>7</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>2064920</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>3</v>
+      </c>
+      <c r="B102">
+        <v>7</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>1827585</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>3</v>
+      </c>
+      <c r="B103">
+        <v>7</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>2</v>
+      </c>
+      <c r="E103">
+        <v>1639996</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>3</v>
+      </c>
+      <c r="B104">
+        <v>7</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>2049370</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>3</v>
+      </c>
+      <c r="B105">
+        <v>7</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+      <c r="E105">
+        <v>1813778</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>3</v>
+      </c>
+      <c r="B106">
+        <v>7</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
+      <c r="E106">
+        <v>1626737</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>3</v>
+      </c>
+      <c r="B107">
+        <v>7</v>
+      </c>
+      <c r="C107">
+        <v>2</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>2040389</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>3</v>
+      </c>
+      <c r="B108">
+        <v>7</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>1805577</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>3</v>
+      </c>
+      <c r="B109">
+        <v>7</v>
+      </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109">
+        <v>2</v>
+      </c>
+      <c r="E109">
+        <v>1618961</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>3</v>
+      </c>
+      <c r="B110">
+        <v>8</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>5643586</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>3</v>
+      </c>
+      <c r="B111">
+        <v>8</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111">
+        <v>5235328</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>3</v>
+      </c>
+      <c r="B112">
+        <v>8</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>2</v>
+      </c>
+      <c r="E112">
+        <v>4917178</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>3</v>
+      </c>
+      <c r="B113">
+        <v>8</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>5566232</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>3</v>
+      </c>
+      <c r="B114">
+        <v>8</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+      <c r="E114">
+        <v>5161165</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>3</v>
+      </c>
+      <c r="B115">
+        <v>8</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <v>2</v>
+      </c>
+      <c r="E115">
+        <v>4845004</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>3</v>
+      </c>
+      <c r="B116">
+        <v>8</v>
+      </c>
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>5515285</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>3</v>
+      </c>
+      <c r="B117">
+        <v>8</v>
+      </c>
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <v>5111888</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>3</v>
+      </c>
+      <c r="B118">
+        <v>8</v>
+      </c>
+      <c r="C118">
+        <v>2</v>
+      </c>
+      <c r="D118">
+        <v>2</v>
+      </c>
+      <c r="E118">
+        <v>4797080</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>3</v>
+      </c>
+      <c r="B119">
+        <v>9</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>12789513</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>3</v>
+      </c>
+      <c r="B120">
+        <v>9</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <v>12274353</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>3</v>
+      </c>
+      <c r="B121">
+        <v>9</v>
+      </c>
+      <c r="C121">
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>2</v>
+      </c>
+      <c r="E121">
+        <v>11856126</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>3</v>
+      </c>
+      <c r="B122">
+        <v>9</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>12525360</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>3</v>
+      </c>
+      <c r="B123">
+        <v>9</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <v>12013252</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>3</v>
+      </c>
+      <c r="B124">
+        <v>9</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+      <c r="D124">
+        <v>2</v>
+      </c>
+      <c r="E124">
+        <v>11598651</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>3</v>
+      </c>
+      <c r="B125">
+        <v>9</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>12336655</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>3</v>
+      </c>
+      <c r="B126">
+        <v>9</v>
+      </c>
+      <c r="C126">
+        <v>2</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="E126">
+        <v>11826286</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>3</v>
+      </c>
+      <c r="B127">
+        <v>9</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
+      <c r="D127">
+        <v>2</v>
+      </c>
+      <c r="E127">
+        <v>11413942</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>3</v>
+      </c>
+      <c r="B128">
+        <v>10</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>25179014</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>3</v>
+      </c>
+      <c r="B129">
+        <v>10</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <v>24632200</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>3</v>
+      </c>
+      <c r="B130">
+        <v>10</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
+      </c>
+      <c r="E130">
+        <v>24200287</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>3</v>
+      </c>
+      <c r="B131">
+        <v>10</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131">
+        <v>24483981</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>3</v>
+      </c>
+      <c r="B132">
+        <v>10</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132">
+        <v>23939952</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>3</v>
+      </c>
+      <c r="B133">
+        <v>10</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+      <c r="D133">
+        <v>2</v>
+      </c>
+      <c r="E133">
+        <v>23513019</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>3</v>
+      </c>
+      <c r="B134">
+        <v>10</v>
+      </c>
+      <c r="C134">
+        <v>2</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134">
+        <v>23961293</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>3</v>
+      </c>
+      <c r="B135">
+        <v>10</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="E135">
+        <v>23418913</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>3</v>
+      </c>
+      <c r="B136">
+        <v>10</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+      <c r="D136">
+        <v>2</v>
+      </c>
+      <c r="E136">
+        <v>22994918</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>3</v>
+      </c>
+      <c r="B137">
+        <v>11</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>41325018</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>3</v>
+      </c>
+      <c r="B138">
+        <v>11</v>
+      </c>
+      <c r="C138">
+        <v>0</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138">
+        <v>41325018</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>3</v>
+      </c>
+      <c r="B139">
+        <v>11</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139">
+        <v>2</v>
+      </c>
+      <c r="E139">
+        <v>41325018</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>3</v>
+      </c>
+      <c r="B140">
+        <v>11</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>39962340</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>3</v>
+      </c>
+      <c r="B141">
+        <v>11</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141">
+        <v>39962340</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>3</v>
+      </c>
+      <c r="B142">
+        <v>11</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <v>2</v>
+      </c>
+      <c r="E142">
+        <v>39962340</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>3</v>
+      </c>
+      <c r="B143">
+        <v>11</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>38906203</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>3</v>
+      </c>
+      <c r="B144">
+        <v>11</v>
+      </c>
+      <c r="C144">
+        <v>2</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>38906203</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>3</v>
+      </c>
+      <c r="B145">
+        <v>11</v>
+      </c>
+      <c r="C145">
+        <v>2</v>
+      </c>
+      <c r="D145">
+        <v>2</v>
+      </c>
+      <c r="E145">
+        <v>38906203</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>3</v>
+      </c>
+      <c r="B146">
+        <v>12</v>
+      </c>
+      <c r="C146">
+        <v>0</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146">
+        <v>41325018</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>3</v>
+      </c>
+      <c r="B147">
+        <v>12</v>
+      </c>
+      <c r="C147">
+        <v>0</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+      <c r="E147">
+        <v>41325018</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>3</v>
+      </c>
+      <c r="B148">
+        <v>12</v>
+      </c>
+      <c r="C148">
+        <v>0</v>
+      </c>
+      <c r="D148">
+        <v>2</v>
+      </c>
+      <c r="E148">
+        <v>41325018</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>3</v>
+      </c>
+      <c r="B149">
+        <v>12</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>39962340</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>3</v>
+      </c>
+      <c r="B150">
+        <v>12</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>39962340</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>3</v>
+      </c>
+      <c r="B151">
+        <v>12</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+      <c r="D151">
+        <v>2</v>
+      </c>
+      <c r="E151">
+        <v>39962340</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>3</v>
+      </c>
+      <c r="B152">
+        <v>12</v>
+      </c>
+      <c r="C152">
+        <v>2</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>38906203</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>3</v>
+      </c>
+      <c r="B153">
+        <v>12</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+      <c r="E153">
+        <v>38906203</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>3</v>
+      </c>
+      <c r="B154">
+        <v>12</v>
+      </c>
+      <c r="C154">
+        <v>2</v>
+      </c>
+      <c r="D154">
+        <v>2</v>
+      </c>
+      <c r="E154">
+        <v>38906203</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>4</v>
+      </c>
+      <c r="B155">
+        <v>2</v>
+      </c>
+      <c r="C155">
+        <v>2</v>
+      </c>
+      <c r="D155">
+        <v>2</v>
+      </c>
+      <c r="E155">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>4</v>
+      </c>
+      <c r="B156">
+        <v>2</v>
+      </c>
+      <c r="C156">
+        <v>2</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+      <c r="E156">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>4</v>
+      </c>
+      <c r="B157">
+        <v>2</v>
+      </c>
+      <c r="C157">
+        <v>2</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>4</v>
+      </c>
+      <c r="B158">
+        <v>2</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="D158">
+        <v>2</v>
+      </c>
+      <c r="E158">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>4</v>
+      </c>
+      <c r="B159">
+        <v>2</v>
+      </c>
+      <c r="C159">
+        <v>1</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+      <c r="E159">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>4</v>
+      </c>
+      <c r="B160">
+        <v>2</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>4</v>
+      </c>
+      <c r="B161">
+        <v>2</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
+      <c r="D161">
+        <v>2</v>
+      </c>
+      <c r="E161">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>4</v>
+      </c>
+      <c r="B162">
+        <v>2</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+      <c r="E162">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>4</v>
+      </c>
+      <c r="B163">
+        <v>2</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>4</v>
+      </c>
+      <c r="B164">
+        <v>3</v>
+      </c>
+      <c r="C164">
+        <v>2</v>
+      </c>
+      <c r="D164">
+        <v>2</v>
+      </c>
+      <c r="E164">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>4</v>
+      </c>
+      <c r="B165">
+        <v>3</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>7877</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>4</v>
+      </c>
+      <c r="B166">
+        <v>3</v>
+      </c>
+      <c r="C166">
+        <v>2</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166">
+        <v>84661</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>4</v>
+      </c>
+      <c r="B167">
+        <v>3</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167">
+        <v>2</v>
+      </c>
+      <c r="E167">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>4</v>
+      </c>
+      <c r="B168">
+        <v>3</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="E168">
+        <v>7877</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>4</v>
+      </c>
+      <c r="B169">
+        <v>3</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="D169">
+        <v>0</v>
+      </c>
+      <c r="E169">
+        <v>84661</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>4</v>
+      </c>
+      <c r="B170">
+        <v>3</v>
+      </c>
+      <c r="C170">
+        <v>0</v>
+      </c>
+      <c r="D170">
+        <v>2</v>
+      </c>
+      <c r="E170">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>4</v>
+      </c>
+      <c r="B171">
+        <v>3</v>
+      </c>
+      <c r="C171">
+        <v>0</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+      <c r="E171">
+        <v>7877</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>4</v>
+      </c>
+      <c r="B172">
+        <v>3</v>
+      </c>
+      <c r="C172">
+        <v>0</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172">
+        <v>84661</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>4</v>
+      </c>
+      <c r="B173">
+        <v>4</v>
+      </c>
+      <c r="C173">
+        <v>2</v>
+      </c>
+      <c r="D173">
+        <v>2</v>
+      </c>
+      <c r="E173">
+        <v>949335</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>4</v>
+      </c>
+      <c r="B174">
+        <v>4</v>
+      </c>
+      <c r="C174">
+        <v>2</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+      <c r="E174">
+        <v>7158361</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>4</v>
+      </c>
+      <c r="B175">
+        <v>4</v>
+      </c>
+      <c r="C175">
+        <v>2</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>23482823</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>4</v>
+      </c>
+      <c r="B176">
+        <v>4</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+      <c r="D176">
+        <v>2</v>
+      </c>
+      <c r="E176">
+        <v>949335</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>4</v>
+      </c>
+      <c r="B177">
+        <v>4</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177">
+        <v>7158361</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>4</v>
+      </c>
+      <c r="B178">
+        <v>4</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>23482823</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>4</v>
+      </c>
+      <c r="B179">
+        <v>4</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="D179">
+        <v>2</v>
+      </c>
+      <c r="E179">
+        <v>949335</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>4</v>
+      </c>
+      <c r="B180">
+        <v>4</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="D180">
+        <v>1</v>
+      </c>
+      <c r="E180">
+        <v>7158361</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>4</v>
+      </c>
+      <c r="B181">
+        <v>4</v>
+      </c>
+      <c r="C181">
+        <v>0</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+      <c r="E181">
+        <v>23482823</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>4</v>
+      </c>
+      <c r="B182">
+        <v>5</v>
+      </c>
+      <c r="C182">
+        <v>2</v>
+      </c>
+      <c r="D182">
+        <v>2</v>
+      </c>
+      <c r="E182">
+        <v>319026096</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>4</v>
+      </c>
+      <c r="B183">
+        <v>5</v>
+      </c>
+      <c r="C183">
+        <v>2</v>
+      </c>
+      <c r="D183">
+        <v>1</v>
+      </c>
+      <c r="E183">
+        <v>796416424</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E183">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20197,22 +23335,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.1640625" customWidth="1"/>
     <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
@@ -20317,7 +23455,7 @@
         <v>1.7231884100965544E-5</v>
       </c>
       <c r="J7">
-        <f>ABS(H7-O7)</f>
+        <f t="shared" ref="J7:J25" si="0">ABS(H7-O7)</f>
         <v>0</v>
       </c>
       <c r="K7">
@@ -20359,19 +23497,19 @@
         <v>0.85863380508680498</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G50" si="0">F8*20</f>
+        <f t="shared" ref="G8:G50" si="1">F8*20</f>
         <v>17.172676101736101</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:H49" si="1">E8+2</f>
+        <f>E8+2</f>
         <v>13</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I71" si="2">ABS(G8-P8)</f>
+        <f t="shared" ref="I8:I38" si="2">ABS(G8-P8)</f>
         <v>1.6665547502014988E-5</v>
       </c>
       <c r="J8">
-        <f>ABS(H8-O8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K8">
@@ -20413,11 +23551,11 @@
         <v>0.85863380508680498</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.172676101736101</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f>E9+2</f>
         <v>10</v>
       </c>
       <c r="I9">
@@ -20425,7 +23563,7 @@
         <v>1.6665547502014988E-5</v>
       </c>
       <c r="J9">
-        <f>ABS(H9-O9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K9">
@@ -20467,11 +23605,11 @@
         <v>0.65694352493194097</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.13887049863882</v>
       </c>
       <c r="H10">
-        <f t="shared" si="1"/>
+        <f>E10+2</f>
         <v>37</v>
       </c>
       <c r="I10">
@@ -20479,7 +23617,7 @@
         <v>1.5236304019339286E-5</v>
       </c>
       <c r="J10">
-        <f>ABS(H10-O10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K10">
@@ -20521,11 +23659,11 @@
         <v>0.65694352493194097</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.13887049863882</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
+        <f>E11+2</f>
         <v>32</v>
       </c>
       <c r="I11">
@@ -20533,7 +23671,7 @@
         <v>1.5156532720439486E-5</v>
       </c>
       <c r="J11">
-        <f>ABS(H11-O11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K11">
@@ -20575,11 +23713,11 @@
         <v>0.65694352493194097</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.13887049863882</v>
       </c>
       <c r="H12">
-        <f t="shared" si="1"/>
+        <f>E12+2</f>
         <v>29</v>
       </c>
       <c r="I12">
@@ -20587,7 +23725,7 @@
         <v>1.4474028720457E-5</v>
       </c>
       <c r="J12">
-        <f>ABS(H12-O12)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K12">
@@ -20629,11 +23767,11 @@
         <v>0.65694352493194097</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.13887049863882</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
+        <f>E13+2</f>
         <v>27</v>
       </c>
       <c r="I13">
@@ -20641,7 +23779,7 @@
         <v>1.4939268119462668E-5</v>
       </c>
       <c r="J13">
-        <f>ABS(H13-O13)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K13">
@@ -20683,11 +23821,11 @@
         <v>4.0307225413361597E-2</v>
       </c>
       <c r="G14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80614450826723194</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
+        <f>E14+2</f>
         <v>59</v>
       </c>
       <c r="I14">
@@ -20695,7 +23833,7 @@
         <v>1.0809384969334701E-6</v>
       </c>
       <c r="J14">
-        <f>ABS(H14-O14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K14">
@@ -20737,11 +23875,11 @@
         <v>4.0307225413361597E-2</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80614450826723194</v>
       </c>
       <c r="H15">
-        <f t="shared" si="1"/>
+        <f>E15+2</f>
         <v>56</v>
       </c>
       <c r="I15">
@@ -20749,7 +23887,7 @@
         <v>1.0809384969334701E-6</v>
       </c>
       <c r="J15">
-        <f>ABS(H15-O15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K15">
@@ -20791,11 +23929,11 @@
         <v>4.0307225413361597E-2</v>
       </c>
       <c r="G16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80614450826723194</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
+        <f>E16+2</f>
         <v>54</v>
       </c>
       <c r="I16">
@@ -20803,7 +23941,7 @@
         <v>1.0752791329560196E-6</v>
       </c>
       <c r="J16">
-        <f>ABS(H16-O16)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K16">
@@ -20845,11 +23983,11 @@
         <v>4.0307225413361597E-2</v>
       </c>
       <c r="G17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.80614450826723194</v>
       </c>
       <c r="H17">
-        <f t="shared" si="1"/>
+        <f>E17+2</f>
         <v>53</v>
       </c>
       <c r="I17">
@@ -20857,7 +23995,7 @@
         <v>1.0756133229650189E-6</v>
       </c>
       <c r="J17">
-        <f>ABS(H17-O17)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K17">
@@ -20899,11 +24037,11 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H18">
-        <f t="shared" si="1"/>
+        <f>E18+2</f>
         <v>76</v>
       </c>
       <c r="I18">
@@ -20911,7 +24049,7 @@
         <v>0</v>
       </c>
       <c r="J18">
-        <f>ABS(H18-O18)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K18">
@@ -20953,11 +24091,11 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H19">
-        <f t="shared" si="1"/>
+        <f>E19+2</f>
         <v>75</v>
       </c>
       <c r="I19">
@@ -20965,7 +24103,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <f>ABS(H19-O19)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K19">
@@ -21007,11 +24145,11 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H20">
-        <f t="shared" si="1"/>
+        <f>E20+2</f>
         <v>73</v>
       </c>
       <c r="I20">
@@ -21019,7 +24157,7 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <f>ABS(H20-O20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K20">
@@ -21061,11 +24199,11 @@
         <v>0</v>
       </c>
       <c r="G21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H21">
-        <f t="shared" si="1"/>
+        <f>E21+2</f>
         <v>72</v>
       </c>
       <c r="I21">
@@ -21073,7 +24211,7 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <f>ABS(H21-O21)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K21">
@@ -21115,11 +24253,11 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H22">
-        <f t="shared" si="1"/>
+        <f>E22+2</f>
         <v>76</v>
       </c>
       <c r="I22">
@@ -21127,7 +24265,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <f>ABS(H22-O22)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K22">
@@ -21169,11 +24307,11 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H23">
-        <f t="shared" si="1"/>
+        <f>E23+2</f>
         <v>75</v>
       </c>
       <c r="I23">
@@ -21181,7 +24319,7 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <f>ABS(H23-O23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K23">
@@ -21223,11 +24361,11 @@
         <v>0</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H24">
-        <f t="shared" si="1"/>
+        <f>E24+2</f>
         <v>73</v>
       </c>
       <c r="I24">
@@ -21235,7 +24373,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <f>ABS(H24-O24)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K24">
@@ -21277,11 +24415,11 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H25">
-        <f t="shared" si="1"/>
+        <f>E25+2</f>
         <v>72</v>
       </c>
       <c r="I25">
@@ -21289,7 +24427,7 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <f>ABS(H25-O25)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K25">
@@ -21331,11 +24469,11 @@
         <v>0.85138298515770605</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.027659703154121</v>
       </c>
       <c r="H26">
-        <f t="shared" si="1"/>
+        <f>E26+2</f>
         <v>1188</v>
       </c>
       <c r="I26">
@@ -21343,7 +24481,7 @@
         <v>1.6662452519966564E-5</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26:J47" si="3">ABS(H26-O26)</f>
+        <f t="shared" ref="J26:J38" si="3">ABS(H26-O26)</f>
         <v>0</v>
       </c>
       <c r="K26">
@@ -21386,11 +24524,11 @@
         <v>0.85138298515770605</v>
       </c>
       <c r="G27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.027659703154121</v>
       </c>
       <c r="H27">
-        <f t="shared" si="1"/>
+        <f>E27+2</f>
         <v>358</v>
       </c>
       <c r="I27">
@@ -21438,19 +24576,19 @@
         <v>99</v>
       </c>
       <c r="F28">
-        <v>0.85120279622033201</v>
+        <v>0.85138298515770605</v>
       </c>
       <c r="G28">
-        <f t="shared" si="0"/>
-        <v>17.024055924406639</v>
+        <f t="shared" si="1"/>
+        <v>17.027659703154121</v>
       </c>
       <c r="H28">
-        <f t="shared" si="1"/>
+        <f>E28+2</f>
         <v>101</v>
       </c>
       <c r="I28">
         <f t="shared" si="2"/>
-        <v>3.5877662360626061E-3</v>
+        <v>1.6012511419916109E-5</v>
       </c>
       <c r="J28">
         <f t="shared" si="3"/>
@@ -21496,11 +24634,11 @@
         <v>0.66196066943017196</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.239213388603439</v>
       </c>
       <c r="H29">
-        <f t="shared" si="1"/>
+        <f>E29+2</f>
         <v>16836</v>
       </c>
       <c r="I29">
@@ -21551,11 +24689,11 @@
         <v>0.66196066943017196</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.239213388603439</v>
       </c>
       <c r="H30">
-        <f t="shared" si="1"/>
+        <f>E30+2</f>
         <v>9830</v>
       </c>
       <c r="I30">
@@ -21606,11 +24744,11 @@
         <v>0.66196066943017196</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.239213388603439</v>
       </c>
       <c r="H31">
-        <f t="shared" si="1"/>
+        <f>E31+2</f>
         <v>4598</v>
       </c>
       <c r="I31">
@@ -21661,11 +24799,11 @@
         <v>0.66191975073806797</v>
       </c>
       <c r="G32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13.238395014761359</v>
       </c>
       <c r="H32">
-        <f t="shared" si="1"/>
+        <f>E32+2</f>
         <v>1986</v>
       </c>
       <c r="I32">
@@ -21720,7 +24858,7 @@
         <v>8.5913878125994803</v>
       </c>
       <c r="H33">
-        <f t="shared" si="1"/>
+        <f>E33+2</f>
         <v>124374</v>
       </c>
       <c r="I33">
@@ -21771,11 +24909,11 @@
         <v>0.42956939062997401</v>
       </c>
       <c r="G34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.5913878125994803</v>
       </c>
       <c r="H34">
-        <f t="shared" si="1"/>
+        <f>E34+2</f>
         <v>92078</v>
       </c>
       <c r="I34">
@@ -21826,11 +24964,11 @@
         <v>0.42956939062997401</v>
       </c>
       <c r="G35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.5913878125994803</v>
       </c>
       <c r="H35">
-        <f t="shared" si="1"/>
+        <f>E35+2</f>
         <v>65899</v>
       </c>
       <c r="I35">
@@ -21881,7 +25019,7 @@
         <v>0.19453624851315501</v>
       </c>
       <c r="G36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8907249702631002</v>
       </c>
       <c r="H36">
@@ -21936,11 +25074,11 @@
         <v>0.19453624851315501</v>
       </c>
       <c r="G37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8907249702631002</v>
       </c>
       <c r="H37">
-        <f t="shared" si="1"/>
+        <f>E37+2</f>
         <v>489027</v>
       </c>
       <c r="I37">
@@ -21991,11 +25129,11 @@
         <v>0.19453624851315501</v>
       </c>
       <c r="G38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8907249702631002</v>
       </c>
       <c r="H38">
-        <f t="shared" si="1"/>
+        <f>E38+2</f>
         <v>405128</v>
       </c>
       <c r="I38">
@@ -22046,15 +25184,15 @@
         <v>4.18598094971964E-2</v>
       </c>
       <c r="G39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83719618994392797</v>
       </c>
       <c r="H39">
-        <f t="shared" si="1"/>
+        <f>E39+2</f>
         <v>2064920</v>
       </c>
       <c r="I39">
-        <f t="shared" ref="I39:I50" si="4">ABS(G39-P39)</f>
+        <f t="shared" ref="I39:I44" si="4">ABS(G39-P39)</f>
         <v>5.4908651692109345E-7</v>
       </c>
       <c r="J39">
@@ -22101,22 +25239,35 @@
         <v>4.18598094971964E-2</v>
       </c>
       <c r="G40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83719618994392797</v>
       </c>
       <c r="H40">
-        <f t="shared" si="1"/>
+        <f>E40+2</f>
         <v>1813777</v>
-      </c>
-      <c r="I40">
-        <f t="shared" si="4"/>
-        <v>0.83719618994392797</v>
       </c>
       <c r="J40">
         <f t="shared" si="5"/>
-        <v>1813777</v>
-      </c>
-      <c r="Q40" s="4"/>
+        <v>13808</v>
+      </c>
+      <c r="K40">
+        <v>3</v>
+      </c>
+      <c r="L40">
+        <v>7</v>
+      </c>
+      <c r="M40" t="s">
+        <v>23</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>1827585</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -22138,22 +25289,35 @@
         <v>4.18598094971964E-2</v>
       </c>
       <c r="G41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83719618994392797</v>
       </c>
       <c r="H41">
-        <f t="shared" si="1"/>
+        <f>E41+2</f>
         <v>1618959</v>
-      </c>
-      <c r="I41">
-        <f t="shared" si="4"/>
-        <v>0.83719618994392797</v>
       </c>
       <c r="J41">
         <f t="shared" si="5"/>
-        <v>1618959</v>
-      </c>
-      <c r="Q41" s="4"/>
+        <v>21037</v>
+      </c>
+      <c r="K41">
+        <v>3</v>
+      </c>
+      <c r="L41">
+        <v>7</v>
+      </c>
+      <c r="M41" t="s">
+        <v>23</v>
+      </c>
+      <c r="N41">
+        <v>2</v>
+      </c>
+      <c r="O41">
+        <v>1639996</v>
+      </c>
+      <c r="Q41" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42">
@@ -22171,26 +25335,39 @@
       <c r="E42">
         <v>5643584</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="4">
         <v>2.0156432845151902E-3</v>
       </c>
       <c r="G42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.0312865690303804E-2</v>
       </c>
       <c r="H42">
-        <f t="shared" si="1"/>
+        <f>E42+2</f>
         <v>5643586</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="4"/>
-        <v>4.0312865690303804E-2</v>
       </c>
       <c r="J42">
         <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>3</v>
+      </c>
+      <c r="L42">
+        <v>8</v>
+      </c>
+      <c r="M42" t="s">
+        <v>23</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
         <v>5643586</v>
       </c>
-      <c r="Q42" s="4"/>
+      <c r="Q42" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43">
@@ -22208,15 +25385,15 @@
       <c r="E43">
         <v>5161162</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="4">
         <v>2.0156432845151902E-3</v>
       </c>
       <c r="G43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.0312865690303804E-2</v>
       </c>
       <c r="H43">
-        <f t="shared" si="1"/>
+        <f>E43+2</f>
         <v>5161164</v>
       </c>
       <c r="I43">
@@ -22263,15 +25440,15 @@
       <c r="E44">
         <v>4797076</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="4">
         <v>2.0156432845151902E-3</v>
       </c>
       <c r="G44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.0312865690303804E-2</v>
       </c>
       <c r="H44">
-        <f t="shared" si="1"/>
+        <f>E44+2</f>
         <v>4797078</v>
       </c>
       <c r="I44">
@@ -22321,20 +25498,34 @@
         <v>3.7091897410257201E-6</v>
       </c>
       <c r="G45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4183794820514409E-5</v>
       </c>
       <c r="H45">
-        <f t="shared" si="1"/>
+        <f>E45+2</f>
         <v>12789513</v>
-      </c>
-      <c r="I45">
-        <f t="shared" si="4"/>
-        <v>7.4183794820514409E-5</v>
       </c>
       <c r="J45">
         <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+      <c r="L45">
+        <v>9</v>
+      </c>
+      <c r="M45" t="s">
+        <v>23</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
         <v>12789513</v>
+      </c>
+      <c r="Q45" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
@@ -22357,20 +25548,34 @@
         <v>3.7091897410257201E-6</v>
       </c>
       <c r="G46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4183794820514409E-5</v>
       </c>
       <c r="H46">
-        <f t="shared" si="1"/>
+        <f>E46+2</f>
         <v>12013251</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="4"/>
-        <v>7.4183794820514409E-5</v>
       </c>
       <c r="J46">
         <f t="shared" si="5"/>
-        <v>12013251</v>
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>3</v>
+      </c>
+      <c r="L46">
+        <v>9</v>
+      </c>
+      <c r="M46" t="s">
+        <v>23</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <v>12013252</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
@@ -22393,20 +25598,34 @@
         <v>3.7091897410257201E-6</v>
       </c>
       <c r="G47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4183794820514409E-5</v>
       </c>
       <c r="H47">
-        <f t="shared" si="1"/>
+        <f>E47+2</f>
         <v>11413940</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="4"/>
-        <v>7.4183794820514409E-5</v>
       </c>
       <c r="J47">
         <f t="shared" si="5"/>
-        <v>11413940</v>
+        <v>2</v>
+      </c>
+      <c r="K47">
+        <v>3</v>
+      </c>
+      <c r="L47">
+        <v>9</v>
+      </c>
+      <c r="M47" t="s">
+        <v>23</v>
+      </c>
+      <c r="N47">
+        <v>2</v>
+      </c>
+      <c r="O47">
+        <v>11413942</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
@@ -22429,23 +25648,37 @@
         <v>3.7321372076390899E-13</v>
       </c>
       <c r="G48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4642744152781792E-12</v>
       </c>
       <c r="H48">
-        <f t="shared" si="1"/>
+        <f>E48+2</f>
         <v>25179014</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="4"/>
-        <v>7.4642744152781792E-12</v>
       </c>
       <c r="J48">
         <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>3</v>
+      </c>
+      <c r="L48">
+        <v>10</v>
+      </c>
+      <c r="M48" t="s">
+        <v>23</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
         <v>25179014</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="Q48" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>3</v>
       </c>
@@ -22465,23 +25698,37 @@
         <v>3.7321372076390899E-13</v>
       </c>
       <c r="G49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4642744152781792E-12</v>
       </c>
       <c r="H49">
-        <f t="shared" si="1"/>
+        <f>E49+2</f>
         <v>23939951</v>
-      </c>
-      <c r="I49">
-        <f t="shared" si="4"/>
-        <v>7.4642744152781792E-12</v>
       </c>
       <c r="J49">
         <f t="shared" si="5"/>
-        <v>23939951</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>3</v>
+      </c>
+      <c r="L49">
+        <v>10</v>
+      </c>
+      <c r="M49" t="s">
+        <v>23</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>23939952</v>
+      </c>
+      <c r="Q49" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>3</v>
       </c>
@@ -22501,31 +25748,44 @@
         <v>3.7321372076390899E-13</v>
       </c>
       <c r="G50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.4642744152781792E-12</v>
       </c>
       <c r="H50">
         <f>E50+2</f>
         <v>22994916</v>
       </c>
-      <c r="I50">
-        <f t="shared" si="4"/>
-        <v>7.4642744152781792E-12</v>
-      </c>
       <c r="J50">
         <f t="shared" si="5"/>
-        <v>22994916</v>
+        <v>2</v>
+      </c>
+      <c r="K50">
+        <v>3</v>
+      </c>
+      <c r="L50">
+        <v>10</v>
+      </c>
+      <c r="M50" t="s">
+        <v>23</v>
+      </c>
+      <c r="N50">
+        <v>2</v>
+      </c>
+      <c r="O50">
+        <v>22994918</v>
+      </c>
+      <c r="Q50" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A6:P50">
-    <sortState ref="A7:P50">
-      <sortCondition ref="A7:A50"/>
-      <sortCondition ref="B7:B50"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A6:Q50"/>
+  <sortState ref="A7:F50">
+    <sortCondition ref="A7:A50"/>
+    <sortCondition ref="B7:B50"/>
+  </sortState>
   <conditionalFormatting sqref="I7:I102">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.0001</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add 4x4 test results
</commit_message>
<xml_diff>
--- a/data/tabulate.xlsx
+++ b/data/tabulate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -20,19 +20,19 @@
     <sheet name="layer_tabulate" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">layer_tabulate!$A$6:$Q$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">layer_tabulate!$A$6:$Q$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">tabulate!$A$1:$J$87</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">tabulate_native!$A$1:$E$183</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">tabulate_new!$A$1:$M$207</definedName>
-    <definedName name="layer_tabulate" localSheetId="5">layer_tabulate!$A$6:$F$50</definedName>
+    <definedName name="layer_tabulate" localSheetId="5">layer_tabulate!$A$6:$F$52</definedName>
     <definedName name="tabulate" localSheetId="1">tabulate!$A$1:$F$20</definedName>
     <definedName name="tabulate_native" localSheetId="3">tabulate_native!$A$1:$E$183</definedName>
     <definedName name="tabulate_new" localSheetId="2">tabulate_new!$A$1:$M$207</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId7"/>
-    <pivotCache cacheId="3" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -76,7 +76,7 @@
     </textPr>
   </connection>
   <connection id="3" name="tabulate_native" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/john/ex/twenty_48/data/tabulate_native.csv" tab="0" comma="1">
+    <textPr fileType="mac" sourceFile="/Users/john/ex/twenty_48/data/layer_tabulate.csv" tab="0" comma="1">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="48">
   <si>
     <t>board_size</t>
   </si>
@@ -256,10 +256,33 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -282,10 +305,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -297,11 +322,64 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3810,7 +3888,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:S13" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
@@ -3951,7 +4029,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:D33" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -11298,8 +11376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M207"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="I206" sqref="I206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19816,8 +19894,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E183"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="E136" sqref="E136"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E109" activeCellId="1" sqref="E105 E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23337,10 +23415,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q50"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23447,7 +23525,7 @@
         <v>17.172676101736101</v>
       </c>
       <c r="H7">
-        <f>E7+2</f>
+        <f t="shared" ref="H7:H52" si="0">E7+2</f>
         <v>17</v>
       </c>
       <c r="I7">
@@ -23455,7 +23533,7 @@
         <v>1.7231884100965544E-5</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:J25" si="0">ABS(H7-O7)</f>
+        <f t="shared" ref="J7:J25" si="1">ABS(H7-O7)</f>
         <v>0</v>
       </c>
       <c r="K7">
@@ -23497,19 +23575,19 @@
         <v>0.85863380508680498</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G50" si="1">F8*20</f>
+        <f t="shared" ref="G8:G52" si="2">F8*20</f>
         <v>17.172676101736101</v>
       </c>
       <c r="H8">
-        <f>E8+2</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I38" si="2">ABS(G8-P8)</f>
+        <f t="shared" ref="I8:I38" si="3">ABS(G8-P8)</f>
         <v>1.6665547502014988E-5</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K8">
@@ -23551,19 +23629,19 @@
         <v>0.85863380508680498</v>
       </c>
       <c r="G9">
+        <f t="shared" si="2"/>
+        <v>17.172676101736101</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>1.6665547502014988E-5</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="1"/>
-        <v>17.172676101736101</v>
-      </c>
-      <c r="H9">
-        <f>E9+2</f>
-        <v>10</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="2"/>
-        <v>1.6665547502014988E-5</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K9">
@@ -23605,19 +23683,19 @@
         <v>0.65694352493194097</v>
       </c>
       <c r="G10">
+        <f t="shared" si="2"/>
+        <v>13.13887049863882</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>1.5236304019339286E-5</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="1"/>
-        <v>13.13887049863882</v>
-      </c>
-      <c r="H10">
-        <f>E10+2</f>
-        <v>37</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="2"/>
-        <v>1.5236304019339286E-5</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K10">
@@ -23659,19 +23737,19 @@
         <v>0.65694352493194097</v>
       </c>
       <c r="G11">
+        <f t="shared" si="2"/>
+        <v>13.13887049863882</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>1.5156532720439486E-5</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="1"/>
-        <v>13.13887049863882</v>
-      </c>
-      <c r="H11">
-        <f>E11+2</f>
-        <v>32</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="2"/>
-        <v>1.5156532720439486E-5</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K11">
@@ -23713,19 +23791,19 @@
         <v>0.65694352493194097</v>
       </c>
       <c r="G12">
+        <f t="shared" si="2"/>
+        <v>13.13887049863882</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>1.4474028720457E-5</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="1"/>
-        <v>13.13887049863882</v>
-      </c>
-      <c r="H12">
-        <f>E12+2</f>
-        <v>29</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="2"/>
-        <v>1.4474028720457E-5</v>
-      </c>
-      <c r="J12">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K12">
@@ -23767,19 +23845,19 @@
         <v>0.65694352493194097</v>
       </c>
       <c r="G13">
+        <f t="shared" si="2"/>
+        <v>13.13887049863882</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>1.4939268119462668E-5</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="1"/>
-        <v>13.13887049863882</v>
-      </c>
-      <c r="H13">
-        <f>E13+2</f>
-        <v>27</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="2"/>
-        <v>1.4939268119462668E-5</v>
-      </c>
-      <c r="J13">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K13">
@@ -23821,19 +23899,19 @@
         <v>4.0307225413361597E-2</v>
       </c>
       <c r="G14">
+        <f t="shared" si="2"/>
+        <v>0.80614450826723194</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>1.0809384969334701E-6</v>
+      </c>
+      <c r="J14">
         <f t="shared" si="1"/>
-        <v>0.80614450826723194</v>
-      </c>
-      <c r="H14">
-        <f>E14+2</f>
-        <v>59</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="2"/>
-        <v>1.0809384969334701E-6</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K14">
@@ -23875,19 +23953,19 @@
         <v>4.0307225413361597E-2</v>
       </c>
       <c r="G15">
+        <f t="shared" si="2"/>
+        <v>0.80614450826723194</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>1.0809384969334701E-6</v>
+      </c>
+      <c r="J15">
         <f t="shared" si="1"/>
-        <v>0.80614450826723194</v>
-      </c>
-      <c r="H15">
-        <f>E15+2</f>
-        <v>56</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="2"/>
-        <v>1.0809384969334701E-6</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K15">
@@ -23929,19 +24007,19 @@
         <v>4.0307225413361597E-2</v>
       </c>
       <c r="G16">
+        <f t="shared" si="2"/>
+        <v>0.80614450826723194</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>1.0752791329560196E-6</v>
+      </c>
+      <c r="J16">
         <f t="shared" si="1"/>
-        <v>0.80614450826723194</v>
-      </c>
-      <c r="H16">
-        <f>E16+2</f>
-        <v>54</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="2"/>
-        <v>1.0752791329560196E-6</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K16">
@@ -23983,19 +24061,19 @@
         <v>4.0307225413361597E-2</v>
       </c>
       <c r="G17">
+        <f t="shared" si="2"/>
+        <v>0.80614450826723194</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>1.0756133229650189E-6</v>
+      </c>
+      <c r="J17">
         <f t="shared" si="1"/>
-        <v>0.80614450826723194</v>
-      </c>
-      <c r="H17">
-        <f>E17+2</f>
-        <v>53</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="2"/>
-        <v>1.0756133229650189E-6</v>
-      </c>
-      <c r="J17">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="K17">
@@ -24037,19 +24115,19 @@
         <v>0</v>
       </c>
       <c r="G18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <f>E18+2</f>
-        <v>76</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K18">
@@ -24091,19 +24169,19 @@
         <v>0</v>
       </c>
       <c r="G19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <f>E19+2</f>
-        <v>75</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K19">
@@ -24145,19 +24223,19 @@
         <v>0</v>
       </c>
       <c r="G20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J20">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <f>E20+2</f>
-        <v>73</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K20">
@@ -24199,19 +24277,19 @@
         <v>0</v>
       </c>
       <c r="G21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J21">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <f>E21+2</f>
-        <v>72</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J21">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K21">
@@ -24253,19 +24331,19 @@
         <v>0</v>
       </c>
       <c r="G22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <f>E22+2</f>
-        <v>76</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K22">
@@ -24307,19 +24385,19 @@
         <v>0</v>
       </c>
       <c r="G23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <f>E23+2</f>
-        <v>75</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K23">
@@ -24361,19 +24439,19 @@
         <v>0</v>
       </c>
       <c r="G24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J24">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <f>E24+2</f>
-        <v>73</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K24">
@@ -24415,19 +24493,19 @@
         <v>0</v>
       </c>
       <c r="G25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <f>E25+2</f>
-        <v>72</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K25">
@@ -24469,19 +24547,19 @@
         <v>0.85138298515770605</v>
       </c>
       <c r="G26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17.027659703154121</v>
       </c>
       <c r="H26">
-        <f>E26+2</f>
+        <f t="shared" si="0"/>
         <v>1188</v>
       </c>
       <c r="I26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6662452519966564E-5</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26:J38" si="3">ABS(H26-O26)</f>
+        <f t="shared" ref="J26:J38" si="4">ABS(H26-O26)</f>
         <v>0</v>
       </c>
       <c r="K26">
@@ -24524,19 +24602,19 @@
         <v>0.85138298515770605</v>
       </c>
       <c r="G27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17.027659703154121</v>
       </c>
       <c r="H27">
-        <f>E27+2</f>
+        <f t="shared" si="0"/>
         <v>358</v>
       </c>
       <c r="I27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6303115220495101E-5</v>
       </c>
       <c r="J27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="K27">
@@ -24579,19 +24657,19 @@
         <v>0.85138298515770605</v>
       </c>
       <c r="G28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>17.027659703154121</v>
       </c>
       <c r="H28">
-        <f>E28+2</f>
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
       <c r="I28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.6012511419916109E-5</v>
       </c>
       <c r="J28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="K28">
@@ -24634,19 +24712,19 @@
         <v>0.66196066943017196</v>
       </c>
       <c r="G29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.239213388603439</v>
       </c>
       <c r="H29">
-        <f>E29+2</f>
+        <f t="shared" si="0"/>
         <v>16836</v>
       </c>
       <c r="I29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4907866638935729E-5</v>
       </c>
       <c r="J29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K29">
@@ -24689,19 +24767,19 @@
         <v>0.66196066943017196</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.239213388603439</v>
       </c>
       <c r="H30">
-        <f>E30+2</f>
+        <f t="shared" si="0"/>
         <v>9830</v>
       </c>
       <c r="I30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4594525138633685E-5</v>
       </c>
       <c r="J30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K30">
@@ -24744,19 +24822,19 @@
         <v>0.66196066943017196</v>
       </c>
       <c r="G31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.239213388603439</v>
       </c>
       <c r="H31">
-        <f>E31+2</f>
+        <f t="shared" si="0"/>
         <v>4598</v>
       </c>
       <c r="I31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4188388139046992E-5</v>
       </c>
       <c r="J31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K31">
@@ -24799,19 +24877,19 @@
         <v>0.66191975073806797</v>
       </c>
       <c r="G32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.238395014761359</v>
       </c>
       <c r="H32">
-        <f>E32+2</f>
+        <f t="shared" si="0"/>
         <v>1986</v>
       </c>
       <c r="I32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.3880839241601279E-5</v>
       </c>
       <c r="J32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>32</v>
       </c>
       <c r="K32">
@@ -24854,19 +24932,19 @@
         <v>0.42956939062997401</v>
       </c>
       <c r="G33">
-        <f>F33*20</f>
+        <f t="shared" si="2"/>
         <v>8.5913878125994803</v>
       </c>
       <c r="H33">
-        <f>E33+2</f>
+        <f t="shared" si="0"/>
         <v>124374</v>
       </c>
       <c r="I33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2255090849677686E-5</v>
       </c>
       <c r="J33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K33">
@@ -24909,19 +24987,19 @@
         <v>0.42956939062997401</v>
       </c>
       <c r="G34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.5913878125994803</v>
       </c>
       <c r="H34">
-        <f>E34+2</f>
+        <f t="shared" si="0"/>
         <v>92078</v>
       </c>
       <c r="I34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2026099909689947E-5</v>
       </c>
       <c r="J34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K34">
@@ -24964,19 +25042,19 @@
         <v>0.42956939062997401</v>
       </c>
       <c r="G35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.5913878125994803</v>
       </c>
       <c r="H35">
-        <f>E35+2</f>
+        <f t="shared" si="0"/>
         <v>65899</v>
       </c>
       <c r="I35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1784159180905363E-5</v>
       </c>
       <c r="J35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K35">
@@ -25019,19 +25097,19 @@
         <v>0.19453624851315501</v>
       </c>
       <c r="G36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.8907249702631002</v>
       </c>
       <c r="H36">
-        <f>E36+2</f>
+        <f t="shared" si="0"/>
         <v>594048</v>
       </c>
       <c r="I36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.8337805399518743E-6</v>
       </c>
       <c r="J36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K36">
@@ -25074,19 +25152,19 @@
         <v>0.19453624851315501</v>
       </c>
       <c r="G37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.8907249702631002</v>
       </c>
       <c r="H37">
-        <f>E37+2</f>
+        <f t="shared" si="0"/>
         <v>489027</v>
       </c>
       <c r="I37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.6976679001260493E-6</v>
       </c>
       <c r="J37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K37">
@@ -25129,19 +25207,19 @@
         <v>0.19453624851315501</v>
       </c>
       <c r="G38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.8907249702631002</v>
       </c>
       <c r="H38">
-        <f>E38+2</f>
+        <f t="shared" si="0"/>
         <v>405128</v>
       </c>
       <c r="I38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.5541845802339367E-6</v>
       </c>
       <c r="J38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="K38">
@@ -25180,23 +25258,23 @@
       <c r="E39">
         <v>2064918</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="4">
         <v>4.18598094971964E-2</v>
       </c>
       <c r="G39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83719618994392797</v>
       </c>
       <c r="H39">
-        <f>E39+2</f>
+        <f t="shared" si="0"/>
         <v>2064920</v>
       </c>
       <c r="I39">
-        <f t="shared" ref="I39:I44" si="4">ABS(G39-P39)</f>
+        <f t="shared" ref="I39:I52" si="5">ABS(G39-P39)</f>
         <v>5.4908651692109345E-7</v>
       </c>
       <c r="J39">
-        <f t="shared" ref="J39:J50" si="5">ABS(H39-O39)</f>
+        <f t="shared" ref="J39:J52" si="6">ABS(H39-O39)</f>
         <v>0</v>
       </c>
       <c r="K39">
@@ -25235,20 +25313,20 @@
       <c r="E40">
         <v>1813775</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="4">
         <v>4.18598094971964E-2</v>
       </c>
       <c r="G40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83719618994392797</v>
       </c>
       <c r="H40">
-        <f>E40+2</f>
+        <f t="shared" si="0"/>
         <v>1813777</v>
       </c>
       <c r="J40">
-        <f t="shared" si="5"/>
-        <v>13808</v>
+        <f>ABS(H40-O40)</f>
+        <v>1</v>
       </c>
       <c r="K40">
         <v>3</v>
@@ -25263,7 +25341,7 @@
         <v>1</v>
       </c>
       <c r="O40">
-        <v>1827585</v>
+        <v>1813778</v>
       </c>
       <c r="Q40" s="4" t="s">
         <v>47</v>
@@ -25285,20 +25363,20 @@
       <c r="E41">
         <v>1618957</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="4">
         <v>4.18598094971964E-2</v>
       </c>
       <c r="G41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.83719618994392797</v>
       </c>
       <c r="H41">
-        <f>E41+2</f>
+        <f t="shared" si="0"/>
         <v>1618959</v>
       </c>
       <c r="J41">
-        <f t="shared" si="5"/>
-        <v>21037</v>
+        <f t="shared" si="6"/>
+        <v>2</v>
       </c>
       <c r="K41">
         <v>3</v>
@@ -25312,8 +25390,8 @@
       <c r="N41">
         <v>2</v>
       </c>
-      <c r="O41">
-        <v>1639996</v>
+      <c r="O41" s="7">
+        <v>1618961</v>
       </c>
       <c r="Q41" s="4" t="s">
         <v>47</v>
@@ -25339,15 +25417,15 @@
         <v>2.0156432845151902E-3</v>
       </c>
       <c r="G42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0312865690303804E-2</v>
       </c>
       <c r="H42">
-        <f>E42+2</f>
+        <f t="shared" si="0"/>
         <v>5643586</v>
       </c>
       <c r="J42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K42">
@@ -25389,19 +25467,19 @@
         <v>2.0156432845151902E-3</v>
       </c>
       <c r="G43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0312865690303804E-2</v>
       </c>
       <c r="H43">
-        <f>E43+2</f>
+        <f t="shared" si="0"/>
         <v>5161164</v>
       </c>
       <c r="I43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.9332707860568741E-7</v>
       </c>
       <c r="J43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K43">
@@ -25444,19 +25522,19 @@
         <v>2.0156432845151902E-3</v>
       </c>
       <c r="G44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0312865690303804E-2</v>
       </c>
       <c r="H44">
-        <f>E44+2</f>
+        <f t="shared" si="0"/>
         <v>4797078</v>
       </c>
       <c r="I44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.9502228020283905E-7</v>
       </c>
       <c r="J44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K44">
@@ -25498,15 +25576,15 @@
         <v>3.7091897410257201E-6</v>
       </c>
       <c r="G45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.4183794820514409E-5</v>
       </c>
       <c r="H45">
-        <f>E45+2</f>
+        <f t="shared" si="0"/>
         <v>12789513</v>
       </c>
       <c r="J45">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K45">
@@ -25548,15 +25626,15 @@
         <v>3.7091897410257201E-6</v>
       </c>
       <c r="G46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.4183794820514409E-5</v>
       </c>
       <c r="H46">
-        <f>E46+2</f>
+        <f t="shared" si="0"/>
         <v>12013251</v>
       </c>
       <c r="J46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K46">
@@ -25598,15 +25676,15 @@
         <v>3.7091897410257201E-6</v>
       </c>
       <c r="G47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.4183794820514409E-5</v>
       </c>
       <c r="H47">
-        <f>E47+2</f>
+        <f t="shared" si="0"/>
         <v>11413940</v>
       </c>
       <c r="J47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K47">
@@ -25648,15 +25726,15 @@
         <v>3.7321372076390899E-13</v>
       </c>
       <c r="G48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.4642744152781792E-12</v>
       </c>
       <c r="H48">
-        <f>E48+2</f>
+        <f t="shared" si="0"/>
         <v>25179014</v>
       </c>
       <c r="J48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K48">
@@ -25698,15 +25776,15 @@
         <v>3.7321372076390899E-13</v>
       </c>
       <c r="G49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.4642744152781792E-12</v>
       </c>
       <c r="H49">
-        <f>E49+2</f>
+        <f t="shared" si="0"/>
         <v>23939951</v>
       </c>
       <c r="J49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="K49">
@@ -25748,15 +25826,15 @@
         <v>3.7321372076390899E-13</v>
       </c>
       <c r="G50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.4642744152781792E-12</v>
       </c>
       <c r="H50">
-        <f>E50+2</f>
+        <f t="shared" si="0"/>
         <v>22994916</v>
       </c>
       <c r="J50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K50">
@@ -25778,13 +25856,122 @@
         <v>47</v>
       </c>
     </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0.95</v>
+      </c>
+      <c r="E51">
+        <v>84659</v>
+      </c>
+      <c r="F51" s="4">
+        <v>0.84703566571448496</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="2"/>
+        <v>16.940713314289699</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>84661</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="5"/>
+        <v>6.9218499980649995E-6</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>4</v>
+      </c>
+      <c r="L51">
+        <v>3</v>
+      </c>
+      <c r="M51" t="s">
+        <v>22</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>84661</v>
+      </c>
+      <c r="P51">
+        <v>16.940706392439701</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>0.95</v>
+      </c>
+      <c r="E52">
+        <v>8673</v>
+      </c>
+      <c r="F52" s="4">
+        <v>0.84703566571448397</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="2"/>
+        <v>16.940713314289681</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="0"/>
+        <v>8675</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="5"/>
+        <v>8.3104479813300713E-6</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="6"/>
+        <v>798</v>
+      </c>
+      <c r="K52">
+        <v>4</v>
+      </c>
+      <c r="L52">
+        <v>3</v>
+      </c>
+      <c r="M52" t="s">
+        <v>22</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <v>7877</v>
+      </c>
+      <c r="P52">
+        <v>16.9407050038417</v>
+      </c>
+      <c r="Q52" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A6:Q50"/>
-  <sortState ref="A7:F50">
-    <sortCondition ref="A7:A50"/>
-    <sortCondition ref="B7:B50"/>
+  <autoFilter ref="A6:Q52"/>
+  <sortState ref="A7:F54">
+    <sortCondition ref="A7:A54"/>
+    <sortCondition ref="B7:B54"/>
   </sortState>
-  <conditionalFormatting sqref="I7:I102">
+  <conditionalFormatting sqref="I7:I100">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.0001</formula>
     </cfRule>

</xml_diff>